<commit_message>
Specs für Leonids Laptop
</commit_message>
<xml_diff>
--- a/Testdokumentation/Integrationstests.xlsx
+++ b/Testdokumentation/Integrationstests.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Testdokumentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4593F66D-E2F8-4ABA-B8FD-2ACA45CF5598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Tests"/>
-    <sheet r:id="rId2" sheetId="2" name="Gerätespecs"/>
+    <sheet name="Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Gerätespecs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
   <si>
     <t>Leonid Surface</t>
   </si>
@@ -510,13 +516,21 @@
   </si>
   <si>
     <t>Die Startansicht wird angezeigt</t>
+  </si>
+  <si>
+    <t>Leonid Laptop</t>
+  </si>
+  <si>
+    <t>Ubuntu 22.04.3</t>
+  </si>
+  <si>
+    <t>Firefox for Ubuntu 121.0 (64 Bit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -566,32 +580,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -602,10 +613,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -643,71 +654,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -735,7 +746,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -758,11 +769,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -771,13 +782,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -787,7 +798,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -796,7 +807,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -805,7 +816,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -813,10 +824,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -881,7 +892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -889,1235 +900,1118 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="98.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="145.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="98.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="145.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="5" t="s">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="1" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="1" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="1" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="5" t="s">
+    <row r="44" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>33</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="1" t="s">
+    </row>
+    <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="1" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="5" t="s">
+    <row r="56" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="1" t="s">
+    </row>
+    <row r="59" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="1" t="s">
+    </row>
+    <row r="60" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="1" t="s">
+    </row>
+    <row r="62" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>73</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="1" t="s">
+    </row>
+    <row r="65" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>86</v>
       </c>
-      <c r="B65" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="1" t="s">
+    </row>
+    <row r="66" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="5" t="s">
+    <row r="67" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B68" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="1" t="s">
+    </row>
+    <row r="69" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="1" t="s">
+    </row>
+    <row r="70" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="1" t="s">
+    </row>
+    <row r="71" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="1" t="s">
+    </row>
+    <row r="72" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="1" t="s">
+    </row>
+    <row r="73" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="1" t="s">
+    </row>
+    <row r="74" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>90</v>
       </c>
-      <c r="B74" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="1" t="s">
+    </row>
+    <row r="75" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="1" t="s">
+    </row>
+    <row r="76" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="1" t="s">
+    </row>
+    <row r="77" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>59</v>
       </c>
-      <c r="B77" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="1" t="s">
+    </row>
+    <row r="78" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="5" t="s">
+    <row r="79" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="1" t="s">
+    </row>
+    <row r="81" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
-      <c r="A82" s="1" t="s">
+    </row>
+    <row r="82" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>48</v>
       </c>
-      <c r="B82" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
-      <c r="A83" s="1" t="s">
+    </row>
+    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>94</v>
       </c>
-      <c r="B83" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
-      <c r="A84" s="1" t="s">
+    </row>
+    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>95</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
-      <c r="A86" s="5" t="s">
+    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B86" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
-      <c r="A87" s="1" t="s">
+    </row>
+    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="1" t="s">
+    </row>
+    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>48</v>
       </c>
-      <c r="B88" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="1" t="s">
+    </row>
+    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>98</v>
       </c>
-      <c r="B89" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
-      <c r="A90" s="1" t="s">
+    </row>
+    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
-      <c r="A92" s="5" t="s">
+    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B92" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="1" t="s">
+    </row>
+    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
-      <c r="A94" s="1" t="s">
+    </row>
+    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>48</v>
       </c>
-      <c r="B94" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
-      <c r="A95" s="1" t="s">
+    </row>
+    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>100</v>
       </c>
-      <c r="B95" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="1" t="s">
+    </row>
+    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="5" t="s">
+    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B98" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="1" t="s">
+    </row>
+    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>103</v>
       </c>
-      <c r="B99" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
-      <c r="A100" s="1" t="s">
+    </row>
+    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>48</v>
       </c>
-      <c r="B100" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
-      <c r="A101" s="1" t="s">
+    </row>
+    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>104</v>
       </c>
-      <c r="B101" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
-      <c r="A102" s="1" t="s">
+    </row>
+    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>95</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
-      <c r="A104" s="5" t="s">
+    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B104" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
-      <c r="A105" s="1" t="s">
+    </row>
+    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>103</v>
       </c>
-      <c r="B105" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
-      <c r="A106" s="1" t="s">
+    </row>
+    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>48</v>
       </c>
-      <c r="B106" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
-      <c r="A107" s="1" t="s">
+    </row>
+    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
-      <c r="A108" s="1" t="s">
+    </row>
+    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>95</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
-      <c r="A110" s="5" t="s">
+    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B110" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
-      <c r="A111" s="1" t="s">
+    </row>
+    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>103</v>
       </c>
-      <c r="B111" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
-      <c r="A112" s="1" t="s">
+    </row>
+    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>48</v>
       </c>
-      <c r="B112" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
-      <c r="A113" s="1" t="s">
+    </row>
+    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>109</v>
       </c>
-      <c r="B113" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
-      <c r="A114" s="1" t="s">
+    </row>
+    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>95</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
-      <c r="A116" s="5" t="s">
+    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B116" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
-      <c r="A117" s="1" t="s">
+    </row>
+    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>111</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>33</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>114</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>116</v>
       </c>
-      <c r="B120" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
-      <c r="A121" s="1" t="s">
+    </row>
+    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>81</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" t="s">
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>41</v>
       </c>
-      <c r="B122" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
-      <c r="A123" s="1" t="s">
+    </row>
+    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>81</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" t="s">
         <v>118</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>41</v>
       </c>
-      <c r="B124" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
-      <c r="A125" s="1" t="s">
+    </row>
+    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>81</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" t="s">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>119</v>
       </c>
-      <c r="B126" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
-      <c r="A127" s="1" t="s">
+    </row>
+    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>120</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" t="s">
         <v>121</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>122</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" t="s">
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>41</v>
       </c>
-      <c r="B129" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
-      <c r="A130" s="1" t="s">
+    </row>
+    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>123</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" t="s">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
-      <c r="A132" s="5" t="s">
+    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B132" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
-      <c r="A133" s="5"/>
-      <c r="B133" s="1" t="s">
+    </row>
+    <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+      <c r="B133" t="s">
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>126</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" t="s">
         <v>127</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>128</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" t="s">
         <v>129</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>130</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" t="s">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>132</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" t="s">
         <v>133</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>134</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" t="s">
         <v>135</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>126</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>136</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" t="s">
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>130</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" t="s">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>138</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" t="s">
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>134</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" t="s">
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>141</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" t="s">
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>143</v>
       </c>
-      <c r="B145" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
-      <c r="A146" s="1" t="s">
+    </row>
+    <row r="146" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>144</v>
       </c>
-      <c r="B146" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
-      <c r="A147" s="1" t="s">
+    </row>
+    <row r="147" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>145</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" t="s">
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
-      <c r="A149" s="5" t="s">
+    <row r="148" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B149" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
-      <c r="A150" s="1" t="s">
+    </row>
+    <row r="150" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>148</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" t="s">
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>150</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" t="s">
         <v>151</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>33</v>
       </c>
-      <c r="B152" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
-      <c r="A153" s="1" t="s">
+    </row>
+    <row r="153" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>152</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" t="s">
         <v>153</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>154</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" t="s">
         <v>155</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
-      <c r="A156" s="5" t="s">
+    <row r="155" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B156" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
-      <c r="A157" s="1" t="s">
+    </row>
+    <row r="157" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>148</v>
       </c>
-      <c r="B157" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
-      <c r="A158" s="1" t="s">
+    </row>
+    <row r="158" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>157</v>
       </c>
-      <c r="B158" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
-      <c r="A159" s="1" t="s">
+    </row>
+    <row r="159" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>44</v>
       </c>
-      <c r="B159" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
-      <c r="A160" s="1" t="s">
+    </row>
+    <row r="160" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>47</v>
       </c>
-      <c r="B160" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
-      <c r="A161" s="1" t="s">
+    </row>
+    <row r="161" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>33</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" t="s">
         <v>158</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
-      <c r="A163" s="5" t="s">
+    <row r="162" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B163" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
-      <c r="A164" s="1" t="s">
+    </row>
+    <row r="164" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>160</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" t="s">
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>44</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>162</v>
       </c>
-      <c r="B166" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
-      <c r="A167" s="1" t="s">
+    </row>
+    <row r="167" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>39</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" t="s">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>41</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>39</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" t="s">
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
-      <c r="A170" s="1" t="s">
+    <row r="170" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>44</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" t="s">
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
-      <c r="A171" s="1" t="s">
+    <row r="171" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>47</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B171" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
-      <c r="A172" s="1" t="s">
+    <row r="172" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>162</v>
       </c>
-      <c r="B172" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
-      <c r="A173" s="1" t="s">
+    </row>
+    <row r="173" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>39</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" t="s">
         <v>164</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
-      <c r="A174" s="1" t="s">
+    <row r="174" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>27</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B174" t="s">
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
-      <c r="A175" s="1" t="s">
+    <row r="175" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>47</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B175" t="s">
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
-      <c r="A176" s="1" t="s">
+    <row r="176" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>162</v>
       </c>
-      <c r="B176" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
-      <c r="A177" s="1" t="s">
+    </row>
+    <row r="177" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>39</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" t="s">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
-      <c r="A178" s="1" t="s">
+    <row r="178" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>41</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
-      <c r="A179" s="1" t="s">
+    <row r="179" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>39</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2127,168 +2021,178 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="24">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrationstests Fehler behoben bzw. verfeinert
</commit_message>
<xml_diff>
--- a/Testdokumentation/Integrationstests.xlsx
+++ b/Testdokumentation/Integrationstests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Testdokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Testdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA05490D-AC38-45D4-B4B4-A432AF4E84A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18410DFD-A1D0-42D2-82A8-818A09D0398A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>Der Nutzer wählt im "Spiel"-Menü für beide Spieler die KI "KI-Elimination" aus und startet das Spiel.</t>
   </si>
   <si>
-    <t>Der Spiel/Graph-Bildschirm wird angezeigt</t>
-  </si>
-  <si>
     <t>Der Nutzer klickt so lange auf das "nächster Zug"-Feld, bis das Spiel vorbei ist.</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>Das Spielergebnis wird angezeigt und zwei Buttons "Belohnen" und "Überspringen". Im Graph werden die Kanten des Pfads vom letzten Knoten (welcher dem Spielfeld entspricht) zum Wurzelknoten hervorgehoben. Die dazu passenden Labels ändern ihre Farbe auf Orange.</t>
   </si>
   <si>
-    <t>Die beiden Buttons werden durch einen Button "Weiter" ersetzt. Der Pfad ist nicht mehr hervorgehoben.</t>
-  </si>
-  <si>
     <t>Das KI-Übersichtsfenster wird angezeigt. Darin sind drei Kis mit ihren Namen aufgelistet.</t>
   </si>
   <si>
@@ -396,9 +390,6 @@
     <t>Der Nutzer wählt das Navigations-Element "KIs" aus.</t>
   </si>
   <si>
-    <t>In der Graphansicht werden alle Label in Magenta angezeigt. Sie haben Werte zwischen 3 und 9. Ein Pfad (die History) ist hervorgehoben.</t>
-  </si>
-  <si>
     <t>Die Magenta-Label werden blau. Die Label entlang der History bleiben grün und haben jetzt Werte zwischen 101 und 109.</t>
   </si>
   <si>
@@ -567,9 +558,6 @@
     <t>Der Graph rutscht zurück rechts neben das Spielfeld.</t>
   </si>
   <si>
-    <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Über dem Spielfeld steht "X Mensch" und "O KI-Elimination". Der Graph zeigt das leere Feld und zeigt die drei Spielfelder mit jeweils einem Kreuz besetzt an (besetzt sind jeweils unterschiedlich Feld 1, 2 und 3). Das leere Feld hat jeweils eine Verbindung zu den anderen drei Spielfeldern. Diesen Graph nennen wir "Graph im Ausgangszustand".</t>
-  </si>
-  <si>
     <t>Die Gewichte des Graphen ändern sich, falls kein Unentschieden stattgefunden hat. Das geänderte Gewicht ist jetzt eine 0 und wird grün angezeigt. Die dazugehörige Kante ist gestrichelt. Alle 1en werden blau angezeigt.</t>
   </si>
   <si>
@@ -579,9 +567,6 @@
     <t>Test: Zwei KIs - Weight-Toggle, Belohnung beider Eliminations-Kis</t>
   </si>
   <si>
-    <t>Im Graph wird oben links ein Toggle-Switch angezeigt. Links daneben steht "X", rechts daneben "O". Der Thumb des Toggle-Switchs ist links platziert. Alle Gewichte sind rot, bis auf die Gewichte der tatsächlich getätigten Züge, welche orange markiert sind. Außerdem sind die Kantenpfeile dieser Züge hervorgehoben.</t>
-  </si>
-  <si>
     <t>Der Thumb des Toggle-Switch wechselt nach rechts. Alle Gewichte im Graph, die vorher rot waren, sind jetzt blau.</t>
   </si>
   <si>
@@ -618,9 +603,6 @@
     <t>Der Einstellungen-Bildschirm wird angezeigt. Die beiden Checkboxes sind immer noch mit einem Haken versehen.</t>
   </si>
   <si>
-    <t>Der Nutzer deaktiviert im Einstellungen-Bildschirm die Optionen "Automatische Belohnung" und "Start überspringen" und spielt ein weitere Spiel bis zum Ende.</t>
-  </si>
-  <si>
     <t>Der Nutzer deaktiviert die Option "Automatische Belohnung", wechselt in den Spielmodus und spielt ein Spiel zu Ende.</t>
   </si>
   <si>
@@ -649,6 +631,24 @@
   </si>
   <si>
     <t>*Belohnung der Rückführungs-KI, Gewichte-Reset*</t>
+  </si>
+  <si>
+    <t>Es wird in die Spielansicht gewechselt. Das Spielfeld ist leer. Über dem Spielfeld steht "X Mensch" und "O KI-Elimination". Der Graph zeigt das leere Feld und zeigt die drei Spielfelder mit jeweils einem Kreuz besetzt an (besetzt sind jeweils unterschiedlich Feld 1, 2 und 5). Das leere Feld hat jeweils eine Verbindung zu den anderen drei Spielfeldern. Diesen Graph nennen wir "Graph im Ausgangszustand".</t>
+  </si>
+  <si>
+    <t>Im Graph wird oben links ein Toggle-Switch angezeigt. Links daneben steht "X", rechts daneben "O". Der Thumb des Toggle-Switchs ist links platziert. Alle Gewichte sind rot, bis auf die Gewichte der tatsächlich getätigten Züge, welche orange markiert sind. Außerdem sind die Kantenpfeile der getätigten Züge hervorgehoben.</t>
+  </si>
+  <si>
+    <t>Der Nutzer deaktiviert im Einstellungen-Bildschirm die Option "Start überspringen" und spielt ein weitere Spiel bis zum Ende.</t>
+  </si>
+  <si>
+    <t>Der Spiel/Graph-Bildschirm wird angezeigt.</t>
+  </si>
+  <si>
+    <t>Die beiden Buttons werden durch einen Button "Weiter" ersetzt. Der Pfad ist nicht mehr orange hervorgehoben.</t>
+  </si>
+  <si>
+    <t>In der Graphansicht werden alle Label in Magenta angezeigt. Sie haben Werte zwischen 3 und 9. Ein Pfad (die History) ist orange hervorgehoben.</t>
   </si>
 </sst>
 </file>
@@ -738,10 +738,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1049,38 +1049,38 @@
   </sheetPr>
   <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="98.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="145.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="145.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1104,23 +1104,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1144,55 +1144,55 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1200,285 +1200,285 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
         <v>140</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>144</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" t="s">
         <v>146</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>151</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" t="s">
         <v>153</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>155</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>158</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B49" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>160</v>
       </c>
-      <c r="B45" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>160</v>
+      </c>
+      <c r="B60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>161</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>160</v>
-      </c>
-      <c r="B47" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="B62" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B54" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>169</v>
-      </c>
-      <c r="B55" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B63" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>163</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>165</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B64" t="s">
         <v>173</v>
       </c>
-      <c r="B63" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>175</v>
-      </c>
-      <c r="B64" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>60</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -1526,37 +1526,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>41</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>52</v>
       </c>
@@ -1580,20 +1580,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>54</v>
       </c>
       <c r="B83" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>56</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>41</v>
       </c>
@@ -1609,12 +1609,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>68</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>41</v>
       </c>
@@ -1630,23 +1630,23 @@
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B91" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -1654,15 +1654,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B93" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>41</v>
       </c>
@@ -1670,13 +1670,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>73</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>75</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>78</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>83</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>81</v>
       </c>
@@ -1716,20 +1716,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B102" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>84</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>86</v>
       </c>
@@ -1745,370 +1745,370 @@
         <v>87</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>89</v>
       </c>
       <c r="B109" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B110" t="s">
         <v>91</v>
       </c>
-      <c r="B110" t="s">
+    </row>
+    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B111" t="s">
         <v>93</v>
       </c>
-      <c r="B111" t="s">
+    </row>
+    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>95</v>
       </c>
-      <c r="B112" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    </row>
+    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>99</v>
+      </c>
+      <c r="B115" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>100</v>
-      </c>
-      <c r="B115" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>98</v>
-      </c>
       <c r="B116" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>41</v>
       </c>
       <c r="B117" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>117</v>
+      </c>
+      <c r="B121" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>197</v>
+      </c>
+      <c r="B122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>103</v>
+      </c>
+      <c r="B123" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>104</v>
+      </c>
+      <c r="B124" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>195</v>
+      </c>
+      <c r="B126" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>103</v>
+      </c>
+      <c r="B127" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>108</v>
+      </c>
+      <c r="B128" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>109</v>
+      </c>
+      <c r="B129" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>111</v>
+      </c>
+      <c r="B130" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>112</v>
+      </c>
+      <c r="B131" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>113</v>
+      </c>
+      <c r="B132" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>119</v>
       </c>
-      <c r="B121" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>203</v>
-      </c>
-      <c r="B122" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>105</v>
-      </c>
-      <c r="B123" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>106</v>
-      </c>
-      <c r="B124" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>201</v>
-      </c>
-      <c r="B126" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>105</v>
-      </c>
-      <c r="B127" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>110</v>
-      </c>
-      <c r="B128" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    </row>
+    <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>115</v>
+      </c>
+      <c r="B135" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>111</v>
       </c>
-      <c r="B129" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>113</v>
-      </c>
-      <c r="B130" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>114</v>
-      </c>
-      <c r="B131" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>115</v>
-      </c>
-      <c r="B132" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="B136" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>117</v>
-      </c>
-      <c r="B135" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>113</v>
-      </c>
-      <c r="B136" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
     </row>
-    <row r="164" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
     </row>
-    <row r="186" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
     </row>
-    <row r="198" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
     </row>
-    <row r="209" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
     </row>
-    <row r="221" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
     </row>
-    <row r="227" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
     </row>
-    <row r="233" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
     </row>
-    <row r="239" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
     </row>
-    <row r="245" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2"/>
     </row>
-    <row r="251" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2"/>
     </row>
-    <row r="257" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="2"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="2"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="2"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="2"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="2"/>
     </row>
   </sheetData>
@@ -2128,144 +2128,152 @@
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+    </row>
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7" t="s">
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7" t="s">
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
@@ -2282,14 +2290,6 @@
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
kleine Fehler in Integrationstests gefixt
</commit_message>
<xml_diff>
--- a/Testdokumentation/Integrationstests.xlsx
+++ b/Testdokumentation/Integrationstests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\GitHub\ticTacToeamprojekt\Testdokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Testdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18410DFD-A1D0-42D2-82A8-818A09D0398A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11A7B5-EB6F-40DB-98E3-377AA517E52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Das angeklickte Feld wird mit "O" belegt.</t>
   </si>
   <si>
-    <t>Die Buttons "Play" und "NextMove" sind ausgegraut. Der Graph zeigt keine Gewichte an. Über dem Spielfeld wird "X: Mensch" und "O: Mensch" angezeigt.</t>
-  </si>
-  <si>
     <t>Der Nutzer versucht den Slider zu verschieben.</t>
   </si>
   <si>
@@ -390,9 +387,6 @@
     <t>Der Nutzer wählt das Navigations-Element "KIs" aus.</t>
   </si>
   <si>
-    <t>Die Magenta-Label werden blau. Die Label entlang der History bleiben grün und haben jetzt Werte zwischen 101 und 109.</t>
-  </si>
-  <si>
     <t>Der Nutzer drückt auf "Weiter" und wechselt dann in den "KIs"-Bildschirm.</t>
   </si>
   <si>
@@ -648,7 +642,13 @@
     <t>Die beiden Buttons werden durch einen Button "Weiter" ersetzt. Der Pfad ist nicht mehr orange hervorgehoben.</t>
   </si>
   <si>
-    <t>In der Graphansicht werden alle Label in Magenta angezeigt. Sie haben Werte zwischen 3 und 9. Ein Pfad (die History) ist orange hervorgehoben.</t>
+    <t>In der Graphansicht werden alle Label in Magenta angezeigt. Sie haben Werte zwischen 1 und 9. Ein Pfad (die History) ist orange hervorgehoben.</t>
+  </si>
+  <si>
+    <t>Die Magenta-Label werden blau. Die Label entlang der History bleiben grün und haben jetzt Werte zwischen 101 und 111.</t>
+  </si>
+  <si>
+    <t>Die Buttons "Play" und "NextMove" sind ausgegraut. Der Graph zeigt keine Gewichte an. Über dem Spielfeld wird "X Mensch" und "O Mensch" angezeigt.</t>
   </si>
 </sst>
 </file>
@@ -1049,38 +1049,38 @@
   </sheetPr>
   <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="145.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="145.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1104,23 +1104,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1144,55 +1144,55 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>128</v>
-      </c>
-      <c r="B16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1200,309 +1200,309 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>137</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>139</v>
-      </c>
-      <c r="B25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>141</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" t="s">
         <v>143</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>148</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>152</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="B43" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>155</v>
-      </c>
-      <c r="B43" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>158</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>157</v>
-      </c>
-      <c r="B47" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B49" s="5" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B58" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>162</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>166</v>
-      </c>
-      <c r="B55" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B62" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>160</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>162</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>170</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>172</v>
-      </c>
-      <c r="B64" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>40</v>
       </c>
       <c r="B68" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1518,597 +1518,597 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" t="s">
         <v>48</v>
       </c>
-      <c r="B73" t="s">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>41</v>
       </c>
       <c r="B81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="B82" t="s">
         <v>52</v>
       </c>
-      <c r="B82" t="s">
+    </row>
+    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B83" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>54</v>
       </c>
-      <c r="B83" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    </row>
+    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="B85" t="s">
         <v>56</v>
       </c>
-      <c r="B85" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>67</v>
+      </c>
+      <c r="B88" t="s">
         <v>68</v>
       </c>
-      <c r="B88" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>41</v>
       </c>
       <c r="B89" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>51</v>
+      </c>
+      <c r="B90" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>187</v>
+      </c>
+      <c r="B91" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>52</v>
-      </c>
-      <c r="B90" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>189</v>
-      </c>
-      <c r="B91" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>41</v>
       </c>
       <c r="B92" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>199</v>
+      </c>
+      <c r="B93" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>201</v>
-      </c>
-      <c r="B93" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>41</v>
       </c>
       <c r="B94" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>72</v>
+      </c>
+      <c r="B97" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>77</v>
+      </c>
+      <c r="B99" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>82</v>
+      </c>
+      <c r="B100" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>188</v>
+      </c>
+      <c r="B102" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>83</v>
+      </c>
+      <c r="B104" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>73</v>
-      </c>
-      <c r="B97" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>75</v>
-      </c>
-      <c r="B98" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>78</v>
-      </c>
-      <c r="B99" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>83</v>
-      </c>
-      <c r="B100" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>81</v>
-      </c>
-      <c r="B101" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>190</v>
-      </c>
-      <c r="B102" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>89</v>
+      </c>
+      <c r="B110" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>93</v>
+      </c>
+      <c r="B112" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>84</v>
-      </c>
-      <c r="B104" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>86</v>
-      </c>
-      <c r="B105" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>89</v>
-      </c>
-      <c r="B109" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>90</v>
-      </c>
-      <c r="B110" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>92</v>
-      </c>
-      <c r="B111" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>94</v>
       </c>
-      <c r="B112" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    </row>
+    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>98</v>
+      </c>
+      <c r="B115" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>99</v>
-      </c>
-      <c r="B115" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>97</v>
-      </c>
       <c r="B116" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>41</v>
       </c>
       <c r="B117" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>116</v>
+      </c>
+      <c r="B121" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>195</v>
+      </c>
+      <c r="B122" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>102</v>
+      </c>
+      <c r="B123" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>103</v>
+      </c>
+      <c r="B124" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>193</v>
+      </c>
+      <c r="B126" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>102</v>
+      </c>
+      <c r="B127" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>107</v>
+      </c>
+      <c r="B128" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>108</v>
+      </c>
+      <c r="B129" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>110</v>
+      </c>
+      <c r="B130" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>111</v>
+      </c>
+      <c r="B131" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>112</v>
+      </c>
+      <c r="B132" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>117</v>
       </c>
-      <c r="B121" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>197</v>
-      </c>
-      <c r="B122" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>103</v>
-      </c>
-      <c r="B123" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>104</v>
-      </c>
-      <c r="B124" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>195</v>
-      </c>
-      <c r="B126" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>103</v>
-      </c>
-      <c r="B127" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>108</v>
-      </c>
-      <c r="B128" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>109</v>
-      </c>
-      <c r="B129" t="s">
+    </row>
+    <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>114</v>
+      </c>
+      <c r="B135" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>111</v>
-      </c>
-      <c r="B130" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>112</v>
-      </c>
-      <c r="B131" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>113</v>
-      </c>
-      <c r="B132" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+      <c r="B136" t="s">
         <v>115</v>
       </c>
-      <c r="B135" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>111</v>
-      </c>
-      <c r="B136" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
     </row>
-    <row r="164" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
     </row>
-    <row r="186" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
     </row>
-    <row r="198" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
     </row>
-    <row r="209" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
     </row>
-    <row r="221" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
     </row>
-    <row r="227" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
     </row>
-    <row r="233" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
     </row>
-    <row r="239" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
     </row>
-    <row r="245" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
     </row>
-    <row r="251" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
     </row>
-    <row r="257" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="2"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="2"/>
     </row>
   </sheetData>
@@ -2128,14 +2128,14 @@
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
     </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
     </row>
-    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2237,7 +2237,7 @@
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
-    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2266,14 +2266,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
@@ -2290,6 +2282,14 @@
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>